<commit_message>
un error nuevo reportado
</commit_message>
<xml_diff>
--- a/relevamientoinfo/tofix.xlsx
+++ b/relevamientoinfo/tofix.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\trunk\relevamientoinfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7305" windowHeight="6180"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <r>
       <t>·</t>
@@ -568,12 +573,60 @@
   </si>
   <si>
     <t>COMENT</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>proveedores</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>En Agregar Cuenta - se rompe cuando quiero agregar una cuenta a un proveedor</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -671,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -737,6 +790,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="10"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,7 +1066,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1021,7 +1077,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1242,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>5.2</v>
       </c>
@@ -1496,6 +1552,38 @@
       <c r="G22" s="13" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="22">
+        <v>43228</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="19"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="22">
+        <v>43231</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="24"/>

</xml_diff>